<commit_message>
Added some features and also include some past projects
</commit_message>
<xml_diff>
--- a/DataEngineerTest/Yahoo-Finance-Scrape-2022-12-22.xlsx
+++ b/DataEngineerTest/Yahoo-Finance-Scrape-2022-12-22.xlsx
@@ -481,7 +481,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -511,7 +511,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -541,7 +541,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -571,7 +571,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -601,7 +601,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -631,7 +631,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -661,7 +661,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -691,7 +691,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -721,7 +721,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -751,7 +751,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -781,7 +781,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -811,7 +811,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -841,7 +841,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -871,7 +871,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -901,7 +901,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -931,7 +931,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -961,7 +961,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -991,7 +991,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1021,7 +1021,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1051,7 +1051,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1081,7 +1081,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1111,7 +1111,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1141,7 +1141,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1171,7 +1171,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1201,7 +1201,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1231,7 +1231,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1261,7 +1261,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -1291,7 +1291,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -1321,7 +1321,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -1351,7 +1351,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -1381,7 +1381,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -1411,7 +1411,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -1441,7 +1441,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -1471,7 +1471,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -1501,7 +1501,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -1531,7 +1531,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -1561,7 +1561,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -1591,7 +1591,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -1621,7 +1621,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -1651,7 +1651,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -1681,7 +1681,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -1711,7 +1711,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -1741,7 +1741,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -1771,7 +1771,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -1801,7 +1801,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -1831,7 +1831,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -1861,7 +1861,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -1891,7 +1891,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -1921,7 +1921,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -1951,7 +1951,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -1981,7 +1981,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -2011,7 +2011,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -2041,7 +2041,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -2071,7 +2071,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -2101,7 +2101,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -2131,7 +2131,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -2161,7 +2161,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -2191,7 +2191,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -2221,7 +2221,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -2251,7 +2251,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -2281,7 +2281,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -2311,7 +2311,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -2341,7 +2341,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -2371,7 +2371,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -2401,7 +2401,7 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -2431,7 +2431,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -2461,7 +2461,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -2491,7 +2491,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -2521,7 +2521,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -2551,7 +2551,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -2581,7 +2581,7 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -2611,7 +2611,7 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -2641,7 +2641,7 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -2671,7 +2671,7 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -2701,7 +2701,7 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -2731,7 +2731,7 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -2761,7 +2761,7 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -2791,7 +2791,7 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -2821,7 +2821,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -2851,7 +2851,7 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -2881,7 +2881,7 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -2911,7 +2911,7 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -2941,7 +2941,7 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -2971,7 +2971,7 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -3001,7 +3001,7 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -3031,7 +3031,7 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -3061,7 +3061,7 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -3091,7 +3091,7 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -3121,7 +3121,7 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -3151,7 +3151,7 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -3181,7 +3181,7 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
@@ -3211,7 +3211,7 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
@@ -3241,7 +3241,7 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
@@ -3271,7 +3271,7 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
@@ -3301,7 +3301,7 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
@@ -3331,7 +3331,7 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
@@ -3361,7 +3361,7 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
@@ -3391,7 +3391,7 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
@@ -3421,7 +3421,7 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
@@ -3451,7 +3451,7 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
@@ -3481,7 +3481,7 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
@@ -3511,7 +3511,7 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
@@ -3541,7 +3541,7 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
@@ -3571,7 +3571,7 @@
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
@@ -3601,7 +3601,7 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
@@ -3631,7 +3631,7 @@
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
@@ -3661,7 +3661,7 @@
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
@@ -3691,7 +3691,7 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
@@ -3721,7 +3721,7 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
@@ -3751,7 +3751,7 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
@@ -3781,7 +3781,7 @@
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
@@ -3811,7 +3811,7 @@
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
@@ -3841,7 +3841,7 @@
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
@@ -3871,7 +3871,7 @@
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
@@ -3901,7 +3901,7 @@
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
@@ -3931,7 +3931,7 @@
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
@@ -3961,7 +3961,7 @@
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
@@ -3991,7 +3991,7 @@
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
@@ -4021,7 +4021,7 @@
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
@@ -4051,7 +4051,7 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
@@ -4081,7 +4081,7 @@
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
@@ -4111,7 +4111,7 @@
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
@@ -4141,7 +4141,7 @@
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
@@ -4171,7 +4171,7 @@
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
@@ -4201,7 +4201,7 @@
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F126" t="inlineStr">
@@ -4231,7 +4231,7 @@
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
@@ -4261,7 +4261,7 @@
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
@@ -4291,7 +4291,7 @@
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F129" t="inlineStr">
@@ -4321,7 +4321,7 @@
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
@@ -4351,7 +4351,7 @@
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
@@ -4381,7 +4381,7 @@
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
@@ -4411,7 +4411,7 @@
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
@@ -4441,7 +4441,7 @@
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F134" t="inlineStr">
@@ -4471,7 +4471,7 @@
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F135" t="inlineStr">
@@ -4501,7 +4501,7 @@
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F136" t="inlineStr">
@@ -4531,7 +4531,7 @@
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F137" t="inlineStr">
@@ -4561,7 +4561,7 @@
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F138" t="inlineStr">
@@ -4591,7 +4591,7 @@
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F139" t="inlineStr">
@@ -4621,7 +4621,7 @@
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F140" t="inlineStr">
@@ -4651,7 +4651,7 @@
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F141" t="inlineStr">
@@ -4681,7 +4681,7 @@
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F142" t="inlineStr">
@@ -4711,7 +4711,7 @@
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F143" t="inlineStr">
@@ -4741,7 +4741,7 @@
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F144" t="inlineStr">
@@ -4771,7 +4771,7 @@
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F145" t="inlineStr">
@@ -4801,7 +4801,7 @@
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F146" t="inlineStr">
@@ -4831,7 +4831,7 @@
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F147" t="inlineStr">
@@ -4861,7 +4861,7 @@
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F148" t="inlineStr">
@@ -4891,7 +4891,7 @@
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F149" t="inlineStr">
@@ -4921,7 +4921,7 @@
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F150" t="inlineStr">
@@ -4951,7 +4951,7 @@
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F151" t="inlineStr">
@@ -4981,7 +4981,7 @@
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F152" t="inlineStr">
@@ -5011,7 +5011,7 @@
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F153" t="inlineStr">
@@ -5041,7 +5041,7 @@
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F154" t="inlineStr">
@@ -5071,7 +5071,7 @@
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F155" t="inlineStr">
@@ -5101,7 +5101,7 @@
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F156" t="inlineStr">
@@ -5131,7 +5131,7 @@
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F157" t="inlineStr">
@@ -5161,7 +5161,7 @@
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F158" t="inlineStr">
@@ -5191,7 +5191,7 @@
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F159" t="inlineStr">
@@ -5221,7 +5221,7 @@
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F160" t="inlineStr">
@@ -5251,7 +5251,7 @@
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F161" t="inlineStr">
@@ -5281,7 +5281,7 @@
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F162" t="inlineStr">
@@ -5311,7 +5311,7 @@
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F163" t="inlineStr">
@@ -5341,7 +5341,7 @@
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F164" t="inlineStr">
@@ -5371,7 +5371,7 @@
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F165" t="inlineStr">
@@ -5401,7 +5401,7 @@
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F166" t="inlineStr">
@@ -5431,7 +5431,7 @@
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F167" t="inlineStr">
@@ -5461,7 +5461,7 @@
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F168" t="inlineStr">
@@ -5491,7 +5491,7 @@
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F169" t="inlineStr">
@@ -5521,7 +5521,7 @@
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F170" t="inlineStr">
@@ -5551,7 +5551,7 @@
       </c>
       <c r="E171" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F171" t="inlineStr">
@@ -5581,7 +5581,7 @@
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F172" t="inlineStr">
@@ -5611,7 +5611,7 @@
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F173" t="inlineStr">
@@ -5641,7 +5641,7 @@
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F174" t="inlineStr">
@@ -5671,7 +5671,7 @@
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F175" t="inlineStr">
@@ -5701,7 +5701,7 @@
       </c>
       <c r="E176" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F176" t="inlineStr">
@@ -5731,7 +5731,7 @@
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F177" t="inlineStr">
@@ -5761,7 +5761,7 @@
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F178" t="inlineStr">
@@ -5791,7 +5791,7 @@
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F179" t="inlineStr">
@@ -5821,7 +5821,7 @@
       </c>
       <c r="E180" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F180" t="inlineStr">
@@ -5851,7 +5851,7 @@
       </c>
       <c r="E181" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F181" t="inlineStr">
@@ -5881,7 +5881,7 @@
       </c>
       <c r="E182" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F182" t="inlineStr">
@@ -5911,7 +5911,7 @@
       </c>
       <c r="E183" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F183" t="inlineStr">
@@ -5941,7 +5941,7 @@
       </c>
       <c r="E184" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F184" t="inlineStr">
@@ -5971,7 +5971,7 @@
       </c>
       <c r="E185" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F185" t="inlineStr">
@@ -6001,7 +6001,7 @@
       </c>
       <c r="E186" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F186" t="inlineStr">
@@ -6031,7 +6031,7 @@
       </c>
       <c r="E187" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F187" t="inlineStr">
@@ -6061,7 +6061,7 @@
       </c>
       <c r="E188" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F188" t="inlineStr">
@@ -6091,7 +6091,7 @@
       </c>
       <c r="E189" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F189" t="inlineStr">
@@ -6121,7 +6121,7 @@
       </c>
       <c r="E190" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F190" t="inlineStr">
@@ -6151,7 +6151,7 @@
       </c>
       <c r="E191" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F191" t="inlineStr">
@@ -6181,7 +6181,7 @@
       </c>
       <c r="E192" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F192" t="inlineStr">
@@ -6211,7 +6211,7 @@
       </c>
       <c r="E193" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F193" t="inlineStr">
@@ -6241,7 +6241,7 @@
       </c>
       <c r="E194" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F194" t="inlineStr">
@@ -6271,7 +6271,7 @@
       </c>
       <c r="E195" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F195" t="inlineStr">
@@ -6301,7 +6301,7 @@
       </c>
       <c r="E196" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F196" t="inlineStr">
@@ -6331,7 +6331,7 @@
       </c>
       <c r="E197" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F197" t="inlineStr">
@@ -6361,7 +6361,7 @@
       </c>
       <c r="E198" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F198" t="inlineStr">
@@ -6391,7 +6391,7 @@
       </c>
       <c r="E199" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F199" t="inlineStr">
@@ -6421,7 +6421,7 @@
       </c>
       <c r="E200" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F200" t="inlineStr">
@@ -6451,7 +6451,7 @@
       </c>
       <c r="E201" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F201" t="inlineStr">
@@ -6481,7 +6481,7 @@
       </c>
       <c r="E202" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F202" t="inlineStr">
@@ -6511,7 +6511,7 @@
       </c>
       <c r="E203" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F203" t="inlineStr">
@@ -6541,7 +6541,7 @@
       </c>
       <c r="E204" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F204" t="inlineStr">
@@ -6571,7 +6571,7 @@
       </c>
       <c r="E205" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F205" t="inlineStr">
@@ -6601,7 +6601,7 @@
       </c>
       <c r="E206" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F206" t="inlineStr">
@@ -6631,7 +6631,7 @@
       </c>
       <c r="E207" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F207" t="inlineStr">
@@ -6661,7 +6661,7 @@
       </c>
       <c r="E208" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F208" t="inlineStr">
@@ -6691,7 +6691,7 @@
       </c>
       <c r="E209" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F209" t="inlineStr">
@@ -6721,7 +6721,7 @@
       </c>
       <c r="E210" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F210" t="inlineStr">
@@ -6751,7 +6751,7 @@
       </c>
       <c r="E211" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F211" t="inlineStr">
@@ -6781,7 +6781,7 @@
       </c>
       <c r="E212" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F212" t="inlineStr">
@@ -6811,7 +6811,7 @@
       </c>
       <c r="E213" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F213" t="inlineStr">
@@ -6841,7 +6841,7 @@
       </c>
       <c r="E214" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F214" t="inlineStr">
@@ -6871,7 +6871,7 @@
       </c>
       <c r="E215" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F215" t="inlineStr">
@@ -6901,7 +6901,7 @@
       </c>
       <c r="E216" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F216" t="inlineStr">
@@ -6931,7 +6931,7 @@
       </c>
       <c r="E217" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F217" t="inlineStr">
@@ -6961,7 +6961,7 @@
       </c>
       <c r="E218" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F218" t="inlineStr">
@@ -6991,7 +6991,7 @@
       </c>
       <c r="E219" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F219" t="inlineStr">
@@ -7021,7 +7021,7 @@
       </c>
       <c r="E220" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F220" t="inlineStr">
@@ -7051,7 +7051,7 @@
       </c>
       <c r="E221" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F221" t="inlineStr">
@@ -7081,7 +7081,7 @@
       </c>
       <c r="E222" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F222" t="inlineStr">
@@ -7111,7 +7111,7 @@
       </c>
       <c r="E223" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F223" t="inlineStr">
@@ -7141,7 +7141,7 @@
       </c>
       <c r="E224" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F224" t="inlineStr">
@@ -7171,7 +7171,7 @@
       </c>
       <c r="E225" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F225" t="inlineStr">
@@ -7201,7 +7201,7 @@
       </c>
       <c r="E226" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F226" t="inlineStr">
@@ -7231,7 +7231,7 @@
       </c>
       <c r="E227" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F227" t="inlineStr">
@@ -7261,7 +7261,7 @@
       </c>
       <c r="E228" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F228" t="inlineStr">
@@ -7291,7 +7291,7 @@
       </c>
       <c r="E229" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F229" t="inlineStr">
@@ -7321,7 +7321,7 @@
       </c>
       <c r="E230" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F230" t="inlineStr">
@@ -7351,7 +7351,7 @@
       </c>
       <c r="E231" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F231" t="inlineStr">
@@ -7381,7 +7381,7 @@
       </c>
       <c r="E232" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F232" t="inlineStr">
@@ -7411,7 +7411,7 @@
       </c>
       <c r="E233" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F233" t="inlineStr">
@@ -7441,7 +7441,7 @@
       </c>
       <c r="E234" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F234" t="inlineStr">
@@ -7471,7 +7471,7 @@
       </c>
       <c r="E235" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F235" t="inlineStr">
@@ -7501,7 +7501,7 @@
       </c>
       <c r="E236" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F236" t="inlineStr">
@@ -7531,7 +7531,7 @@
       </c>
       <c r="E237" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F237" t="inlineStr">
@@ -7561,7 +7561,7 @@
       </c>
       <c r="E238" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F238" t="inlineStr">
@@ -7591,7 +7591,7 @@
       </c>
       <c r="E239" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F239" t="inlineStr">
@@ -7621,7 +7621,7 @@
       </c>
       <c r="E240" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F240" t="inlineStr">
@@ -7651,7 +7651,7 @@
       </c>
       <c r="E241" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F241" t="inlineStr">
@@ -7681,7 +7681,7 @@
       </c>
       <c r="E242" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F242" t="inlineStr">
@@ -7711,7 +7711,7 @@
       </c>
       <c r="E243" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F243" t="inlineStr">
@@ -7741,7 +7741,7 @@
       </c>
       <c r="E244" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F244" t="inlineStr">
@@ -7771,7 +7771,7 @@
       </c>
       <c r="E245" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F245" t="inlineStr">
@@ -7801,7 +7801,7 @@
       </c>
       <c r="E246" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F246" t="inlineStr">
@@ -7831,7 +7831,7 @@
       </c>
       <c r="E247" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F247" t="inlineStr">
@@ -7861,7 +7861,7 @@
       </c>
       <c r="E248" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F248" t="inlineStr">
@@ -7891,7 +7891,7 @@
       </c>
       <c r="E249" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F249" t="inlineStr">
@@ -7921,7 +7921,7 @@
       </c>
       <c r="E250" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F250" t="inlineStr">
@@ -7951,7 +7951,7 @@
       </c>
       <c r="E251" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F251" t="inlineStr">
@@ -7981,7 +7981,7 @@
       </c>
       <c r="E252" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F252" t="inlineStr">
@@ -8011,7 +8011,7 @@
       </c>
       <c r="E253" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F253" t="inlineStr">
@@ -8041,7 +8041,7 @@
       </c>
       <c r="E254" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F254" t="inlineStr">
@@ -8071,7 +8071,7 @@
       </c>
       <c r="E255" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F255" t="inlineStr">
@@ -8101,7 +8101,7 @@
       </c>
       <c r="E256" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F256" t="inlineStr">
@@ -8131,7 +8131,7 @@
       </c>
       <c r="E257" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F257" t="inlineStr">
@@ -8161,7 +8161,7 @@
       </c>
       <c r="E258" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F258" t="inlineStr">
@@ -8191,7 +8191,7 @@
       </c>
       <c r="E259" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F259" t="inlineStr">
@@ -8221,7 +8221,7 @@
       </c>
       <c r="E260" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F260" t="inlineStr">
@@ -8251,7 +8251,7 @@
       </c>
       <c r="E261" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F261" t="inlineStr">
@@ -8281,7 +8281,7 @@
       </c>
       <c r="E262" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F262" t="inlineStr">
@@ -8311,7 +8311,7 @@
       </c>
       <c r="E263" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F263" t="inlineStr">
@@ -8341,7 +8341,7 @@
       </c>
       <c r="E264" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F264" t="inlineStr">
@@ -8371,7 +8371,7 @@
       </c>
       <c r="E265" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F265" t="inlineStr">
@@ -8401,7 +8401,7 @@
       </c>
       <c r="E266" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F266" t="inlineStr">
@@ -8431,7 +8431,7 @@
       </c>
       <c r="E267" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F267" t="inlineStr">
@@ -8461,7 +8461,7 @@
       </c>
       <c r="E268" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F268" t="inlineStr">
@@ -8491,7 +8491,7 @@
       </c>
       <c r="E269" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F269" t="inlineStr">
@@ -8521,7 +8521,7 @@
       </c>
       <c r="E270" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F270" t="inlineStr">
@@ -8551,7 +8551,7 @@
       </c>
       <c r="E271" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F271" t="inlineStr">
@@ -8581,7 +8581,7 @@
       </c>
       <c r="E272" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F272" t="inlineStr">
@@ -8611,7 +8611,7 @@
       </c>
       <c r="E273" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F273" t="inlineStr">
@@ -8641,7 +8641,7 @@
       </c>
       <c r="E274" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F274" t="inlineStr">
@@ -8671,7 +8671,7 @@
       </c>
       <c r="E275" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F275" t="inlineStr">
@@ -8701,7 +8701,7 @@
       </c>
       <c r="E276" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F276" t="inlineStr">
@@ -8731,7 +8731,7 @@
       </c>
       <c r="E277" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F277" t="inlineStr">
@@ -8761,7 +8761,7 @@
       </c>
       <c r="E278" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F278" t="inlineStr">
@@ -8791,7 +8791,7 @@
       </c>
       <c r="E279" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F279" t="inlineStr">
@@ -8821,7 +8821,7 @@
       </c>
       <c r="E280" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>9-30-2022</t>
         </is>
       </c>
       <c r="F280" t="inlineStr">
@@ -8851,7 +8851,7 @@
       </c>
       <c r="E281" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F281" t="inlineStr">
@@ -8881,7 +8881,7 @@
       </c>
       <c r="E282" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F282" t="inlineStr">
@@ -8911,7 +8911,7 @@
       </c>
       <c r="E283" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F283" t="inlineStr">
@@ -8941,7 +8941,7 @@
       </c>
       <c r="E284" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F284" t="inlineStr">
@@ -8971,7 +8971,7 @@
       </c>
       <c r="E285" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F285" t="inlineStr">
@@ -9001,7 +9001,7 @@
       </c>
       <c r="E286" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F286" t="inlineStr">
@@ -9031,7 +9031,7 @@
       </c>
       <c r="E287" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F287" t="inlineStr">
@@ -9061,7 +9061,7 @@
       </c>
       <c r="E288" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F288" t="inlineStr">
@@ -9091,7 +9091,7 @@
       </c>
       <c r="E289" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F289" t="inlineStr">
@@ -9121,7 +9121,7 @@
       </c>
       <c r="E290" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F290" t="inlineStr">
@@ -9151,7 +9151,7 @@
       </c>
       <c r="E291" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F291" t="inlineStr">
@@ -9181,7 +9181,7 @@
       </c>
       <c r="E292" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F292" t="inlineStr">
@@ -9211,7 +9211,7 @@
       </c>
       <c r="E293" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F293" t="inlineStr">
@@ -9241,7 +9241,7 @@
       </c>
       <c r="E294" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F294" t="inlineStr">
@@ -9271,7 +9271,7 @@
       </c>
       <c r="E295" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F295" t="inlineStr">
@@ -9301,7 +9301,7 @@
       </c>
       <c r="E296" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F296" t="inlineStr">
@@ -9331,7 +9331,7 @@
       </c>
       <c r="E297" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F297" t="inlineStr">
@@ -9361,7 +9361,7 @@
       </c>
       <c r="E298" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F298" t="inlineStr">
@@ -9391,7 +9391,7 @@
       </c>
       <c r="E299" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F299" t="inlineStr">
@@ -9421,7 +9421,7 @@
       </c>
       <c r="E300" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F300" t="inlineStr">
@@ -9451,7 +9451,7 @@
       </c>
       <c r="E301" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F301" t="inlineStr">
@@ -9481,7 +9481,7 @@
       </c>
       <c r="E302" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F302" t="inlineStr">
@@ -9511,7 +9511,7 @@
       </c>
       <c r="E303" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F303" t="inlineStr">
@@ -9541,7 +9541,7 @@
       </c>
       <c r="E304" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F304" t="inlineStr">
@@ -9571,7 +9571,7 @@
       </c>
       <c r="E305" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F305" t="inlineStr">
@@ -9601,7 +9601,7 @@
       </c>
       <c r="E306" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F306" t="inlineStr">
@@ -9631,7 +9631,7 @@
       </c>
       <c r="E307" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F307" t="inlineStr">
@@ -9661,7 +9661,7 @@
       </c>
       <c r="E308" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F308" t="inlineStr">
@@ -9691,7 +9691,7 @@
       </c>
       <c r="E309" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F309" t="inlineStr">
@@ -9721,7 +9721,7 @@
       </c>
       <c r="E310" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F310" t="inlineStr">
@@ -9751,7 +9751,7 @@
       </c>
       <c r="E311" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F311" t="inlineStr">
@@ -9781,7 +9781,7 @@
       </c>
       <c r="E312" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F312" t="inlineStr">
@@ -9811,7 +9811,7 @@
       </c>
       <c r="E313" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F313" t="inlineStr">
@@ -9841,7 +9841,7 @@
       </c>
       <c r="E314" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F314" t="inlineStr">
@@ -9871,7 +9871,7 @@
       </c>
       <c r="E315" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F315" t="inlineStr">
@@ -9901,7 +9901,7 @@
       </c>
       <c r="E316" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F316" t="inlineStr">
@@ -9931,7 +9931,7 @@
       </c>
       <c r="E317" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F317" t="inlineStr">
@@ -9961,7 +9961,7 @@
       </c>
       <c r="E318" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F318" t="inlineStr">
@@ -9991,7 +9991,7 @@
       </c>
       <c r="E319" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F319" t="inlineStr">
@@ -10021,7 +10021,7 @@
       </c>
       <c r="E320" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F320" t="inlineStr">
@@ -10051,7 +10051,7 @@
       </c>
       <c r="E321" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F321" t="inlineStr">
@@ -10081,7 +10081,7 @@
       </c>
       <c r="E322" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F322" t="inlineStr">
@@ -10111,7 +10111,7 @@
       </c>
       <c r="E323" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F323" t="inlineStr">
@@ -10141,7 +10141,7 @@
       </c>
       <c r="E324" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F324" t="inlineStr">
@@ -10171,7 +10171,7 @@
       </c>
       <c r="E325" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F325" t="inlineStr">
@@ -10201,7 +10201,7 @@
       </c>
       <c r="E326" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F326" t="inlineStr">
@@ -10231,7 +10231,7 @@
       </c>
       <c r="E327" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F327" t="inlineStr">
@@ -10261,7 +10261,7 @@
       </c>
       <c r="E328" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F328" t="inlineStr">
@@ -10291,7 +10291,7 @@
       </c>
       <c r="E329" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F329" t="inlineStr">
@@ -10321,7 +10321,7 @@
       </c>
       <c r="E330" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F330" t="inlineStr">
@@ -10351,7 +10351,7 @@
       </c>
       <c r="E331" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F331" t="inlineStr">
@@ -10381,7 +10381,7 @@
       </c>
       <c r="E332" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F332" t="inlineStr">
@@ -10411,7 +10411,7 @@
       </c>
       <c r="E333" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F333" t="inlineStr">
@@ -10441,7 +10441,7 @@
       </c>
       <c r="E334" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F334" t="inlineStr">
@@ -10471,7 +10471,7 @@
       </c>
       <c r="E335" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F335" t="inlineStr">
@@ -10501,7 +10501,7 @@
       </c>
       <c r="E336" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F336" t="inlineStr">
@@ -10531,7 +10531,7 @@
       </c>
       <c r="E337" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F337" t="inlineStr">
@@ -10561,7 +10561,7 @@
       </c>
       <c r="E338" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F338" t="inlineStr">
@@ -10591,7 +10591,7 @@
       </c>
       <c r="E339" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F339" t="inlineStr">
@@ -10621,7 +10621,7 @@
       </c>
       <c r="E340" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F340" t="inlineStr">
@@ -10651,7 +10651,7 @@
       </c>
       <c r="E341" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F341" t="inlineStr">
@@ -10681,7 +10681,7 @@
       </c>
       <c r="E342" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F342" t="inlineStr">
@@ -10711,7 +10711,7 @@
       </c>
       <c r="E343" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F343" t="inlineStr">
@@ -10741,7 +10741,7 @@
       </c>
       <c r="E344" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F344" t="inlineStr">
@@ -10771,7 +10771,7 @@
       </c>
       <c r="E345" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F345" t="inlineStr">
@@ -10801,7 +10801,7 @@
       </c>
       <c r="E346" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F346" t="inlineStr">
@@ -10831,7 +10831,7 @@
       </c>
       <c r="E347" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F347" t="inlineStr">
@@ -10861,7 +10861,7 @@
       </c>
       <c r="E348" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F348" t="inlineStr">
@@ -10891,7 +10891,7 @@
       </c>
       <c r="E349" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F349" t="inlineStr">
@@ -10921,7 +10921,7 @@
       </c>
       <c r="E350" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F350" t="inlineStr">
@@ -10951,7 +10951,7 @@
       </c>
       <c r="E351" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F351" t="inlineStr">
@@ -10981,7 +10981,7 @@
       </c>
       <c r="E352" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F352" t="inlineStr">
@@ -11011,7 +11011,7 @@
       </c>
       <c r="E353" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F353" t="inlineStr">
@@ -11041,7 +11041,7 @@
       </c>
       <c r="E354" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F354" t="inlineStr">
@@ -11071,7 +11071,7 @@
       </c>
       <c r="E355" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F355" t="inlineStr">
@@ -11101,7 +11101,7 @@
       </c>
       <c r="E356" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F356" t="inlineStr">
@@ -11131,7 +11131,7 @@
       </c>
       <c r="E357" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F357" t="inlineStr">
@@ -11161,7 +11161,7 @@
       </c>
       <c r="E358" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F358" t="inlineStr">
@@ -11191,7 +11191,7 @@
       </c>
       <c r="E359" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F359" t="inlineStr">
@@ -11221,7 +11221,7 @@
       </c>
       <c r="E360" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F360" t="inlineStr">
@@ -11251,7 +11251,7 @@
       </c>
       <c r="E361" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F361" t="inlineStr">
@@ -11281,7 +11281,7 @@
       </c>
       <c r="E362" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F362" t="inlineStr">
@@ -11311,7 +11311,7 @@
       </c>
       <c r="E363" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F363" t="inlineStr">
@@ -11341,7 +11341,7 @@
       </c>
       <c r="E364" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F364" t="inlineStr">
@@ -11371,7 +11371,7 @@
       </c>
       <c r="E365" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F365" t="inlineStr">
@@ -11401,7 +11401,7 @@
       </c>
       <c r="E366" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F366" t="inlineStr">
@@ -11431,7 +11431,7 @@
       </c>
       <c r="E367" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F367" t="inlineStr">
@@ -11461,7 +11461,7 @@
       </c>
       <c r="E368" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F368" t="inlineStr">
@@ -11491,7 +11491,7 @@
       </c>
       <c r="E369" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F369" t="inlineStr">
@@ -11521,7 +11521,7 @@
       </c>
       <c r="E370" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F370" t="inlineStr">
@@ -11551,7 +11551,7 @@
       </c>
       <c r="E371" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F371" t="inlineStr">
@@ -11581,7 +11581,7 @@
       </c>
       <c r="E372" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F372" t="inlineStr">
@@ -11611,7 +11611,7 @@
       </c>
       <c r="E373" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F373" t="inlineStr">
@@ -11641,7 +11641,7 @@
       </c>
       <c r="E374" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F374" t="inlineStr">
@@ -11671,7 +11671,7 @@
       </c>
       <c r="E375" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F375" t="inlineStr">
@@ -11701,7 +11701,7 @@
       </c>
       <c r="E376" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F376" t="inlineStr">
@@ -11731,7 +11731,7 @@
       </c>
       <c r="E377" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F377" t="inlineStr">
@@ -11761,7 +11761,7 @@
       </c>
       <c r="E378" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F378" t="inlineStr">
@@ -11791,7 +11791,7 @@
       </c>
       <c r="E379" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F379" t="inlineStr">
@@ -11821,7 +11821,7 @@
       </c>
       <c r="E380" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F380" t="inlineStr">
@@ -11851,7 +11851,7 @@
       </c>
       <c r="E381" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F381" t="inlineStr">
@@ -11881,7 +11881,7 @@
       </c>
       <c r="E382" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F382" t="inlineStr">
@@ -11911,7 +11911,7 @@
       </c>
       <c r="E383" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F383" t="inlineStr">
@@ -11941,7 +11941,7 @@
       </c>
       <c r="E384" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F384" t="inlineStr">
@@ -11971,7 +11971,7 @@
       </c>
       <c r="E385" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F385" t="inlineStr">
@@ -12001,7 +12001,7 @@
       </c>
       <c r="E386" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F386" t="inlineStr">
@@ -12031,7 +12031,7 @@
       </c>
       <c r="E387" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F387" t="inlineStr">
@@ -12061,7 +12061,7 @@
       </c>
       <c r="E388" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F388" t="inlineStr">
@@ -12091,7 +12091,7 @@
       </c>
       <c r="E389" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F389" t="inlineStr">
@@ -12121,7 +12121,7 @@
       </c>
       <c r="E390" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F390" t="inlineStr">
@@ -12151,7 +12151,7 @@
       </c>
       <c r="E391" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F391" t="inlineStr">
@@ -12181,7 +12181,7 @@
       </c>
       <c r="E392" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F392" t="inlineStr">
@@ -12211,7 +12211,7 @@
       </c>
       <c r="E393" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F393" t="inlineStr">
@@ -12241,7 +12241,7 @@
       </c>
       <c r="E394" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F394" t="inlineStr">
@@ -12271,7 +12271,7 @@
       </c>
       <c r="E395" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F395" t="inlineStr">
@@ -12301,7 +12301,7 @@
       </c>
       <c r="E396" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F396" t="inlineStr">
@@ -12331,7 +12331,7 @@
       </c>
       <c r="E397" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F397" t="inlineStr">
@@ -12361,7 +12361,7 @@
       </c>
       <c r="E398" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F398" t="inlineStr">
@@ -12391,7 +12391,7 @@
       </c>
       <c r="E399" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>6-30-2022</t>
         </is>
       </c>
       <c r="F399" t="inlineStr">
@@ -12421,7 +12421,7 @@
       </c>
       <c r="E400" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F400" t="inlineStr">
@@ -12451,7 +12451,7 @@
       </c>
       <c r="E401" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F401" t="inlineStr">
@@ -12481,7 +12481,7 @@
       </c>
       <c r="E402" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F402" t="inlineStr">
@@ -12511,7 +12511,7 @@
       </c>
       <c r="E403" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F403" t="inlineStr">
@@ -12541,7 +12541,7 @@
       </c>
       <c r="E404" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F404" t="inlineStr">
@@ -12571,7 +12571,7 @@
       </c>
       <c r="E405" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F405" t="inlineStr">
@@ -12601,7 +12601,7 @@
       </c>
       <c r="E406" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F406" t="inlineStr">
@@ -12631,7 +12631,7 @@
       </c>
       <c r="E407" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F407" t="inlineStr">
@@ -12661,7 +12661,7 @@
       </c>
       <c r="E408" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F408" t="inlineStr">
@@ -12691,7 +12691,7 @@
       </c>
       <c r="E409" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F409" t="inlineStr">
@@ -12721,7 +12721,7 @@
       </c>
       <c r="E410" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F410" t="inlineStr">
@@ -12751,7 +12751,7 @@
       </c>
       <c r="E411" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F411" t="inlineStr">
@@ -12781,7 +12781,7 @@
       </c>
       <c r="E412" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F412" t="inlineStr">
@@ -12811,7 +12811,7 @@
       </c>
       <c r="E413" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F413" t="inlineStr">
@@ -12841,7 +12841,7 @@
       </c>
       <c r="E414" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F414" t="inlineStr">
@@ -12871,7 +12871,7 @@
       </c>
       <c r="E415" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F415" t="inlineStr">
@@ -12901,7 +12901,7 @@
       </c>
       <c r="E416" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F416" t="inlineStr">
@@ -12931,7 +12931,7 @@
       </c>
       <c r="E417" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F417" t="inlineStr">
@@ -12961,7 +12961,7 @@
       </c>
       <c r="E418" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F418" t="inlineStr">
@@ -12991,7 +12991,7 @@
       </c>
       <c r="E419" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F419" t="inlineStr">
@@ -13021,7 +13021,7 @@
       </c>
       <c r="E420" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F420" t="inlineStr">
@@ -13051,7 +13051,7 @@
       </c>
       <c r="E421" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F421" t="inlineStr">
@@ -13081,7 +13081,7 @@
       </c>
       <c r="E422" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F422" t="inlineStr">
@@ -13111,7 +13111,7 @@
       </c>
       <c r="E423" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F423" t="inlineStr">
@@ -13141,7 +13141,7 @@
       </c>
       <c r="E424" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F424" t="inlineStr">
@@ -13171,7 +13171,7 @@
       </c>
       <c r="E425" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F425" t="inlineStr">
@@ -13201,7 +13201,7 @@
       </c>
       <c r="E426" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F426" t="inlineStr">
@@ -13231,7 +13231,7 @@
       </c>
       <c r="E427" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F427" t="inlineStr">
@@ -13261,7 +13261,7 @@
       </c>
       <c r="E428" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F428" t="inlineStr">
@@ -13291,7 +13291,7 @@
       </c>
       <c r="E429" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F429" t="inlineStr">
@@ -13321,7 +13321,7 @@
       </c>
       <c r="E430" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F430" t="inlineStr">
@@ -13351,7 +13351,7 @@
       </c>
       <c r="E431" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F431" t="inlineStr">
@@ -13381,7 +13381,7 @@
       </c>
       <c r="E432" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F432" t="inlineStr">
@@ -13411,7 +13411,7 @@
       </c>
       <c r="E433" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F433" t="inlineStr">
@@ -13441,7 +13441,7 @@
       </c>
       <c r="E434" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F434" t="inlineStr">
@@ -13471,7 +13471,7 @@
       </c>
       <c r="E435" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F435" t="inlineStr">
@@ -13501,7 +13501,7 @@
       </c>
       <c r="E436" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F436" t="inlineStr">
@@ -13531,7 +13531,7 @@
       </c>
       <c r="E437" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F437" t="inlineStr">
@@ -13561,7 +13561,7 @@
       </c>
       <c r="E438" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F438" t="inlineStr">
@@ -13591,7 +13591,7 @@
       </c>
       <c r="E439" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F439" t="inlineStr">
@@ -13621,7 +13621,7 @@
       </c>
       <c r="E440" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F440" t="inlineStr">
@@ -13651,7 +13651,7 @@
       </c>
       <c r="E441" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F441" t="inlineStr">
@@ -13681,7 +13681,7 @@
       </c>
       <c r="E442" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F442" t="inlineStr">
@@ -13711,7 +13711,7 @@
       </c>
       <c r="E443" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F443" t="inlineStr">
@@ -13741,7 +13741,7 @@
       </c>
       <c r="E444" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F444" t="inlineStr">
@@ -13771,7 +13771,7 @@
       </c>
       <c r="E445" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F445" t="inlineStr">
@@ -13801,7 +13801,7 @@
       </c>
       <c r="E446" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F446" t="inlineStr">
@@ -13831,7 +13831,7 @@
       </c>
       <c r="E447" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F447" t="inlineStr">
@@ -13861,7 +13861,7 @@
       </c>
       <c r="E448" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F448" t="inlineStr">
@@ -13891,7 +13891,7 @@
       </c>
       <c r="E449" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F449" t="inlineStr">
@@ -13921,7 +13921,7 @@
       </c>
       <c r="E450" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F450" t="inlineStr">
@@ -13951,7 +13951,7 @@
       </c>
       <c r="E451" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F451" t="inlineStr">
@@ -13981,7 +13981,7 @@
       </c>
       <c r="E452" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F452" t="inlineStr">
@@ -14011,7 +14011,7 @@
       </c>
       <c r="E453" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F453" t="inlineStr">
@@ -14041,7 +14041,7 @@
       </c>
       <c r="E454" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F454" t="inlineStr">
@@ -14071,7 +14071,7 @@
       </c>
       <c r="E455" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F455" t="inlineStr">
@@ -14101,7 +14101,7 @@
       </c>
       <c r="E456" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>1-31-2022</t>
         </is>
       </c>
       <c r="F456" t="inlineStr">
@@ -14131,7 +14131,7 @@
       </c>
       <c r="E457" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F457" t="inlineStr">
@@ -14161,7 +14161,7 @@
       </c>
       <c r="E458" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F458" t="inlineStr">
@@ -14191,7 +14191,7 @@
       </c>
       <c r="E459" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F459" t="inlineStr">
@@ -14221,7 +14221,7 @@
       </c>
       <c r="E460" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F460" t="inlineStr">
@@ -14251,7 +14251,7 @@
       </c>
       <c r="E461" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F461" t="inlineStr">
@@ -14281,7 +14281,7 @@
       </c>
       <c r="E462" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F462" t="inlineStr">
@@ -14311,7 +14311,7 @@
       </c>
       <c r="E463" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F463" t="inlineStr">
@@ -14341,7 +14341,7 @@
       </c>
       <c r="E464" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F464" t="inlineStr">
@@ -14371,7 +14371,7 @@
       </c>
       <c r="E465" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F465" t="inlineStr">
@@ -14401,7 +14401,7 @@
       </c>
       <c r="E466" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F466" t="inlineStr">
@@ -14431,7 +14431,7 @@
       </c>
       <c r="E467" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F467" t="inlineStr">
@@ -14461,7 +14461,7 @@
       </c>
       <c r="E468" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F468" t="inlineStr">
@@ -14491,7 +14491,7 @@
       </c>
       <c r="E469" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F469" t="inlineStr">
@@ -14521,7 +14521,7 @@
       </c>
       <c r="E470" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F470" t="inlineStr">
@@ -14551,7 +14551,7 @@
       </c>
       <c r="E471" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F471" t="inlineStr">
@@ -14581,7 +14581,7 @@
       </c>
       <c r="E472" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F472" t="inlineStr">
@@ -14611,7 +14611,7 @@
       </c>
       <c r="E473" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F473" t="inlineStr">
@@ -14641,7 +14641,7 @@
       </c>
       <c r="E474" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F474" t="inlineStr">
@@ -14671,7 +14671,7 @@
       </c>
       <c r="E475" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F475" t="inlineStr">
@@ -14701,7 +14701,7 @@
       </c>
       <c r="E476" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F476" t="inlineStr">
@@ -14731,7 +14731,7 @@
       </c>
       <c r="E477" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F477" t="inlineStr">
@@ -14761,7 +14761,7 @@
       </c>
       <c r="E478" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F478" t="inlineStr">
@@ -14791,7 +14791,7 @@
       </c>
       <c r="E479" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F479" t="inlineStr">
@@ -14821,7 +14821,7 @@
       </c>
       <c r="E480" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F480" t="inlineStr">
@@ -14851,7 +14851,7 @@
       </c>
       <c r="E481" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F481" t="inlineStr">
@@ -14881,7 +14881,7 @@
       </c>
       <c r="E482" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F482" t="inlineStr">
@@ -14911,7 +14911,7 @@
       </c>
       <c r="E483" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F483" t="inlineStr">
@@ -14941,7 +14941,7 @@
       </c>
       <c r="E484" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F484" t="inlineStr">
@@ -14971,7 +14971,7 @@
       </c>
       <c r="E485" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F485" t="inlineStr">
@@ -15001,7 +15001,7 @@
       </c>
       <c r="E486" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F486" t="inlineStr">
@@ -15031,7 +15031,7 @@
       </c>
       <c r="E487" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F487" t="inlineStr">
@@ -15061,7 +15061,7 @@
       </c>
       <c r="E488" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F488" t="inlineStr">
@@ -15091,7 +15091,7 @@
       </c>
       <c r="E489" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F489" t="inlineStr">
@@ -15121,7 +15121,7 @@
       </c>
       <c r="E490" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F490" t="inlineStr">
@@ -15151,7 +15151,7 @@
       </c>
       <c r="E491" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F491" t="inlineStr">
@@ -15181,7 +15181,7 @@
       </c>
       <c r="E492" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F492" t="inlineStr">
@@ -15211,7 +15211,7 @@
       </c>
       <c r="E493" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F493" t="inlineStr">
@@ -15241,7 +15241,7 @@
       </c>
       <c r="E494" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F494" t="inlineStr">
@@ -15271,7 +15271,7 @@
       </c>
       <c r="E495" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F495" t="inlineStr">
@@ -15301,7 +15301,7 @@
       </c>
       <c r="E496" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F496" t="inlineStr">
@@ -15331,7 +15331,7 @@
       </c>
       <c r="E497" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F497" t="inlineStr">
@@ -15361,7 +15361,7 @@
       </c>
       <c r="E498" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F498" t="inlineStr">
@@ -15391,7 +15391,7 @@
       </c>
       <c r="E499" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F499" t="inlineStr">
@@ -15421,7 +15421,7 @@
       </c>
       <c r="E500" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F500" t="inlineStr">
@@ -15451,7 +15451,7 @@
       </c>
       <c r="E501" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F501" t="inlineStr">
@@ -15481,7 +15481,7 @@
       </c>
       <c r="E502" t="inlineStr">
         <is>
-          <t>12-22-2022</t>
+          <t>12-31-2021</t>
         </is>
       </c>
       <c r="F502" t="inlineStr">

</xml_diff>